<commit_message>
general hierarchical classifier code
</commit_message>
<xml_diff>
--- a/Hierarchical Classification Results.xlsx
+++ b/Hierarchical Classification Results.xlsx
@@ -4,12 +4,14 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20225"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="7680" yWindow="0" windowWidth="25800" windowHeight="16360" tabRatio="500"/>
+    <workbookView xWindow="3880" yWindow="0" windowWidth="25600" windowHeight="16060" tabRatio="500" activeTab="4"/>
   </bookViews>
   <sheets>
-    <sheet name="GO" sheetId="1" r:id="rId1"/>
-    <sheet name="GO 5 fold x-validation" sheetId="2" r:id="rId2"/>
-    <sheet name="taxonomy" sheetId="3" r:id="rId3"/>
+    <sheet name="GO-Bayes" sheetId="1" r:id="rId1"/>
+    <sheet name="GO-Bayes 5 fold x-validation" sheetId="2" r:id="rId2"/>
+    <sheet name="GO-SVM" sheetId="4" r:id="rId3"/>
+    <sheet name="GO-SVM 5 fold x-validation" sheetId="5" r:id="rId4"/>
+    <sheet name="taxonomy-Bayes" sheetId="3" r:id="rId5"/>
   </sheets>
   <calcPr calcId="140001" concurrentCalc="0"/>
   <extLst>
@@ -21,10 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="364" uniqueCount="33">
-  <si>
-    <t>Sample Threshold Results</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="417" uniqueCount="35">
   <si>
     <t>Cellular Component</t>
   </si>
@@ -121,6 +120,15 @@
   <si>
     <t>nodes w/ &gt;2 children only</t>
   </si>
+  <si>
+    <t>Uniprot Abstracts</t>
+  </si>
+  <si>
+    <t>Uniprot Abstracts Dataset</t>
+  </si>
+  <si>
+    <t>Nematoda</t>
+  </si>
 </sst>
 </file>
 
@@ -202,8 +210,18 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="87">
+  <cellStyleXfs count="97">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -318,7 +336,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
-  <cellStyles count="87">
+  <cellStyles count="97">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -362,6 +380,11 @@
     <cellStyle name="Followed Hyperlink" xfId="82" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="84" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="86" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="88" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="90" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="92" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="94" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="96" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -405,6 +428,11 @@
     <cellStyle name="Hyperlink" xfId="81" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="83" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="85" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="87" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="89" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="91" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="93" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="95" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -736,8 +764,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M128"/>
   <sheetViews>
-    <sheetView tabSelected="1" showRuler="0" topLeftCell="A44" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
-      <selection activeCell="E120" sqref="E120"/>
+    <sheetView showRuler="0" topLeftCell="A50" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -749,41 +777,41 @@
   <sheetData>
     <row r="1" spans="1:13" s="4" customFormat="1">
       <c r="A1" s="4" t="s">
-        <v>0</v>
+        <v>33</v>
       </c>
     </row>
     <row r="2" spans="1:13" s="7" customFormat="1">
       <c r="A2" s="7" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D2" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="G2" s="7" t="s">
         <v>6</v>
-      </c>
-      <c r="G2" s="7" t="s">
-        <v>7</v>
       </c>
     </row>
     <row r="3" spans="1:13" s="1" customFormat="1">
       <c r="G3" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="4" spans="1:13">
       <c r="A4" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B4">
         <v>0</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E4" s="2">
         <v>0</v>
       </c>
       <c r="F4" s="2"/>
       <c r="G4" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="H4" s="2">
         <v>0</v>
@@ -796,20 +824,20 @@
     </row>
     <row r="5" spans="1:13">
       <c r="A5" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B5">
         <v>3902</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E5" s="2">
         <v>10057</v>
       </c>
       <c r="F5" s="2"/>
       <c r="G5" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="H5" s="2">
         <v>6319</v>
@@ -822,15 +850,15 @@
     </row>
     <row r="6" spans="1:13" s="1" customFormat="1">
       <c r="A6" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="E6" s="3"/>
       <c r="F6" s="3"/>
       <c r="G6" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="H6" s="3">
         <v>0.204035763078878</v>
@@ -846,15 +874,15 @@
     </row>
     <row r="7" spans="1:13">
       <c r="A7" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="E7" s="2"/>
       <c r="F7" s="2"/>
       <c r="G7" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="H7" s="2">
         <v>0.27093682569203698</v>
@@ -867,15 +895,15 @@
     </row>
     <row r="8" spans="1:13">
       <c r="A8" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="E8" s="2"/>
       <c r="F8" s="2"/>
       <c r="G8" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="H8" s="2">
         <v>0.22796059653171</v>
@@ -888,7 +916,7 @@
     </row>
     <row r="9" spans="1:13">
       <c r="A9" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D9" s="1"/>
       <c r="E9" s="2"/>
@@ -904,20 +932,20 @@
     <row r="10" spans="1:13" s="1" customFormat="1"/>
     <row r="11" spans="1:13">
       <c r="A11" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B11">
         <v>3</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E11" s="2">
         <v>3</v>
       </c>
       <c r="F11" s="2"/>
       <c r="G11" s="3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="H11" s="2">
         <v>3</v>
@@ -930,20 +958,20 @@
     </row>
     <row r="12" spans="1:13">
       <c r="A12" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B12">
         <v>1019</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E12" s="2">
         <v>2641</v>
       </c>
       <c r="F12" s="2"/>
       <c r="G12" s="3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="H12" s="2">
         <v>8048</v>
@@ -956,20 +984,20 @@
     </row>
     <row r="13" spans="1:13" s="1" customFormat="1">
       <c r="A13" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B13" s="1">
         <v>0.48576143311547798</v>
       </c>
       <c r="D13" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="E13" s="3">
         <v>0.42389983732683101</v>
       </c>
       <c r="F13" s="3"/>
       <c r="G13" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="H13" s="3">
         <f>(2*H14*H15)/(H14+H15)</f>
@@ -983,20 +1011,20 @@
     </row>
     <row r="14" spans="1:13">
       <c r="A14" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B14">
         <v>0.54709100711506498</v>
       </c>
       <c r="D14" s="3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="E14" s="2">
         <v>0.60370370713948596</v>
       </c>
       <c r="F14" s="2"/>
       <c r="G14" s="3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="H14" s="2">
         <v>0.27093682569203698</v>
@@ -1009,20 +1037,20 @@
     </row>
     <row r="15" spans="1:13">
       <c r="A15" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B15">
         <v>0.43679605836792801</v>
       </c>
       <c r="D15" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="E15" s="2">
         <v>0.40844856585831202</v>
       </c>
       <c r="F15" s="2"/>
       <c r="G15" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="H15" s="2">
         <v>0.22796059653171</v>
@@ -1035,16 +1063,16 @@
     </row>
     <row r="16" spans="1:13">
       <c r="A16" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B16">
         <v>41</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="G16" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="17" spans="1:13">
@@ -1062,20 +1090,20 @@
     </row>
     <row r="18" spans="1:13">
       <c r="A18" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B18">
         <v>5</v>
       </c>
       <c r="D18" s="3" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E18" s="2">
         <v>5</v>
       </c>
       <c r="F18" s="2"/>
       <c r="G18" s="3" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="H18" s="2">
         <v>5</v>
@@ -1088,20 +1116,20 @@
     </row>
     <row r="19" spans="1:13">
       <c r="A19" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B19">
         <v>792</v>
       </c>
       <c r="D19" s="3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E19" s="2">
         <v>1887</v>
       </c>
       <c r="F19" s="2"/>
       <c r="G19" s="3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="H19" s="2"/>
       <c r="I19" s="2"/>
@@ -1112,20 +1140,20 @@
     </row>
     <row r="20" spans="1:13" s="1" customFormat="1">
       <c r="A20" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B20" s="1">
         <v>0.48576143311547798</v>
       </c>
       <c r="D20" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="E20" s="3">
         <v>0.48807197980933698</v>
       </c>
       <c r="F20" s="3"/>
       <c r="G20" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="H20" s="3"/>
       <c r="I20" s="3"/>
@@ -1136,20 +1164,20 @@
     </row>
     <row r="21" spans="1:13">
       <c r="A21" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B21">
         <v>0.54709100711506498</v>
       </c>
       <c r="D21" s="3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="E21" s="2">
         <v>0.62680451482770305</v>
       </c>
       <c r="F21" s="2"/>
       <c r="G21" s="3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="H21" s="2"/>
       <c r="I21" s="2"/>
@@ -1160,20 +1188,20 @@
     </row>
     <row r="22" spans="1:13">
       <c r="A22" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B22">
         <v>0.43679605836792801</v>
       </c>
       <c r="D22" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="E22" s="2">
         <v>0.399622357359323</v>
       </c>
       <c r="F22" s="2"/>
       <c r="G22" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="H22" s="2"/>
       <c r="I22" s="2"/>
@@ -1184,13 +1212,13 @@
     </row>
     <row r="23" spans="1:13">
       <c r="A23" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B23">
         <v>41</v>
       </c>
       <c r="D23" s="3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E23" s="2"/>
       <c r="F23" s="2"/>
@@ -1217,20 +1245,20 @@
     </row>
     <row r="25" spans="1:13">
       <c r="A25" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B25">
         <v>10</v>
       </c>
       <c r="D25" s="3" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E25" s="2">
         <v>10</v>
       </c>
       <c r="F25" s="2"/>
       <c r="G25" s="3" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="H25" s="2">
         <v>10</v>
@@ -1243,20 +1271,20 @@
     </row>
     <row r="26" spans="1:13">
       <c r="A26" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B26">
         <v>565</v>
       </c>
       <c r="D26" s="3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E26" s="2">
         <v>1160</v>
       </c>
       <c r="F26" s="2"/>
       <c r="G26" s="3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="H26" s="2">
         <v>4209</v>
@@ -1269,20 +1297,20 @@
     </row>
     <row r="27" spans="1:13" s="1" customFormat="1">
       <c r="A27" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B27" s="1">
         <v>0.48576143311547798</v>
       </c>
       <c r="D27" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="E27" s="3">
         <v>0.48807333436241201</v>
       </c>
       <c r="F27" s="3"/>
       <c r="G27" s="9" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="H27" s="3">
         <v>0.24896843627107901</v>
@@ -1295,20 +1323,20 @@
     </row>
     <row r="28" spans="1:13">
       <c r="A28" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B28">
         <v>0.54709100711506498</v>
       </c>
       <c r="D28" s="3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="E28" s="2">
         <v>0.62680898294323095</v>
       </c>
       <c r="F28" s="2"/>
       <c r="G28" s="3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="H28" s="2">
         <v>0.29761920043191598</v>
@@ -1321,20 +1349,20 @@
     </row>
     <row r="29" spans="1:13">
       <c r="A29" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B29">
         <v>0.43679605836792801</v>
       </c>
       <c r="D29" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="E29" s="2">
         <v>0.399622357359323</v>
       </c>
       <c r="F29" s="2"/>
       <c r="G29" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="H29" s="2">
         <v>0.21398849023168601</v>
@@ -1347,18 +1375,18 @@
     </row>
     <row r="30" spans="1:13">
       <c r="A30" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B30">
         <v>41</v>
       </c>
       <c r="D30" s="3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E30" s="2"/>
       <c r="F30" s="2"/>
       <c r="G30" s="3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="H30" s="2">
         <v>20</v>
@@ -1384,20 +1412,20 @@
     </row>
     <row r="32" spans="1:13">
       <c r="A32" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B32">
         <v>100</v>
       </c>
       <c r="D32" s="3" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E32" s="2">
         <v>100</v>
       </c>
       <c r="F32" s="2"/>
       <c r="G32" s="3" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="H32" s="2">
         <v>100</v>
@@ -1410,20 +1438,20 @@
     </row>
     <row r="33" spans="1:13">
       <c r="A33" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B33">
         <v>155</v>
       </c>
       <c r="D33" s="3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E33" s="2">
         <v>247</v>
       </c>
       <c r="F33" s="2"/>
       <c r="G33" s="3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="H33" s="2">
         <v>970</v>
@@ -1436,20 +1464,20 @@
     </row>
     <row r="34" spans="1:13" s="1" customFormat="1">
       <c r="A34" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B34" s="1">
         <v>0.48616835187587498</v>
       </c>
       <c r="D34" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="E34" s="3">
         <v>0.48817437148173798</v>
       </c>
       <c r="F34" s="3"/>
       <c r="G34" s="9" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="H34" s="3">
         <v>0.24910208437516501</v>
@@ -1462,20 +1490,20 @@
     </row>
     <row r="35" spans="1:13">
       <c r="A35" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B35">
         <v>0.548124402950247</v>
       </c>
       <c r="D35" s="3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="E35" s="2">
         <v>0.62715704548235196</v>
       </c>
       <c r="F35" s="2"/>
       <c r="G35" s="3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="H35" s="2">
         <v>0.298001453053098</v>
@@ -1488,20 +1516,20 @@
     </row>
     <row r="36" spans="1:13">
       <c r="A36" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B36">
         <v>0.43679605836792801</v>
       </c>
       <c r="D36" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="E36" s="2">
         <v>0.39961639987195302</v>
       </c>
       <c r="F36" s="2"/>
       <c r="G36" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="H36" s="2">
         <v>0.21398849023168601</v>
@@ -1514,20 +1542,20 @@
     </row>
     <row r="37" spans="1:13">
       <c r="A37" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B37">
         <v>41</v>
       </c>
       <c r="D37" s="3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E37" s="2">
         <v>50</v>
       </c>
       <c r="F37" s="2"/>
       <c r="G37" s="3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="H37" s="2">
         <v>20</v>
@@ -1553,20 +1581,20 @@
     </row>
     <row r="39" spans="1:13">
       <c r="A39" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B39">
         <v>150</v>
       </c>
       <c r="D39" s="3" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E39" s="2">
         <v>150</v>
       </c>
       <c r="F39" s="2"/>
       <c r="G39" s="3" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="H39" s="2">
         <v>150</v>
@@ -1579,20 +1607,20 @@
     </row>
     <row r="40" spans="1:13">
       <c r="A40" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B40">
         <v>116</v>
       </c>
       <c r="D40" s="3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E40" s="2">
         <v>184</v>
       </c>
       <c r="F40" s="2"/>
       <c r="G40" s="3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="H40" s="2">
         <v>705</v>
@@ -1605,20 +1633,20 @@
     </row>
     <row r="41" spans="1:13" s="1" customFormat="1">
       <c r="A41" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B41" s="1">
         <v>0.48637052779672801</v>
       </c>
       <c r="D41" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="E41" s="3">
         <v>0.48840285846010301</v>
       </c>
       <c r="F41" s="3"/>
       <c r="G41" s="9" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="H41" s="3">
         <v>0.249392064267002</v>
@@ -1631,20 +1659,20 @@
     </row>
     <row r="42" spans="1:13">
       <c r="A42" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B42">
         <v>0.54879059026371202</v>
       </c>
       <c r="D42" s="3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="E42" s="2">
         <v>0.62841784423852098</v>
       </c>
       <c r="F42" s="2"/>
       <c r="G42" s="3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="H42" s="2">
         <v>0.29883280427546099</v>
@@ -1657,20 +1685,20 @@
     </row>
     <row r="43" spans="1:13">
       <c r="A43" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B43">
         <v>0.43669979874196502</v>
       </c>
       <c r="D43" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="E43" s="2">
         <v>0.39941171101014</v>
       </c>
       <c r="F43" s="2"/>
       <c r="G43" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="H43" s="2">
         <v>0.21398849023168601</v>
@@ -1683,20 +1711,20 @@
     </row>
     <row r="44" spans="1:13">
       <c r="A44" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B44">
         <v>41</v>
       </c>
       <c r="D44" s="3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E44" s="2">
         <v>50</v>
       </c>
       <c r="F44" s="2"/>
       <c r="G44" s="3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="H44" s="2">
         <v>20</v>
@@ -1722,20 +1750,20 @@
     </row>
     <row r="46" spans="1:13">
       <c r="A46" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B46">
         <v>200</v>
       </c>
       <c r="D46" s="3" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E46" s="2">
         <v>200</v>
       </c>
       <c r="F46" s="2"/>
       <c r="G46" s="3" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="H46" s="2">
         <v>200</v>
@@ -1748,20 +1776,20 @@
     </row>
     <row r="47" spans="1:13">
       <c r="A47" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B47">
         <v>97</v>
       </c>
       <c r="D47" s="3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E47" s="2">
         <v>138</v>
       </c>
       <c r="F47" s="2"/>
       <c r="G47" s="3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="H47" s="2"/>
       <c r="I47" s="2"/>
@@ -1772,20 +1800,20 @@
     </row>
     <row r="48" spans="1:13" s="1" customFormat="1">
       <c r="A48" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B48" s="1">
         <v>0.48675278744709499</v>
       </c>
       <c r="D48" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="E48" s="3">
         <v>0.48840285846010301</v>
       </c>
       <c r="F48" s="3"/>
       <c r="G48" s="9" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="H48" s="3"/>
       <c r="I48" s="3"/>
@@ -1796,20 +1824,20 @@
     </row>
     <row r="49" spans="1:13">
       <c r="A49" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B49">
         <v>0.54976489860342004</v>
       </c>
       <c r="D49" s="3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="E49" s="2">
         <v>0.62841784423852098</v>
       </c>
       <c r="F49" s="2"/>
       <c r="G49" s="3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="H49" s="2"/>
       <c r="I49" s="2"/>
@@ -1820,20 +1848,20 @@
     </row>
     <row r="50" spans="1:13">
       <c r="A50" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B50">
         <v>0.43669979874196502</v>
       </c>
       <c r="D50" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="E50" s="2">
         <v>0.39941171101014</v>
       </c>
       <c r="F50" s="2"/>
       <c r="G50" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="H50" s="2"/>
       <c r="I50" s="2"/>
@@ -1844,13 +1872,13 @@
     </row>
     <row r="51" spans="1:13">
       <c r="A51" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B51">
         <v>41</v>
       </c>
       <c r="D51" s="3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E51" s="2">
         <v>50</v>
@@ -1879,20 +1907,20 @@
     </row>
     <row r="53" spans="1:13">
       <c r="A53" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B53">
         <v>250</v>
       </c>
       <c r="D53" s="3" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E53" s="2">
         <v>250</v>
       </c>
       <c r="F53" s="2"/>
       <c r="G53" s="3" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="H53" s="2">
         <v>250</v>
@@ -1905,20 +1933,20 @@
     </row>
     <row r="54" spans="1:13">
       <c r="A54" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B54">
         <v>85</v>
       </c>
       <c r="D54" s="3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E54" s="2">
         <v>129</v>
       </c>
       <c r="F54" s="2"/>
       <c r="G54" s="3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="H54" s="2"/>
       <c r="I54" s="2"/>
@@ -1929,20 +1957,20 @@
     </row>
     <row r="55" spans="1:13" s="1" customFormat="1">
       <c r="A55" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B55" s="1">
         <v>0.48702320940955901</v>
       </c>
       <c r="D55" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="E55" s="3">
         <v>0.488605161251217</v>
       </c>
       <c r="F55" s="3"/>
       <c r="G55" s="9" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="H55" s="3"/>
       <c r="I55" s="3"/>
@@ -1953,20 +1981,20 @@
     </row>
     <row r="56" spans="1:13">
       <c r="A56" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B56">
         <v>0.55078339772073703</v>
       </c>
       <c r="D56" s="3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="E56" s="2">
         <v>0.62913898705262805</v>
       </c>
       <c r="F56" s="2"/>
       <c r="G56" s="3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="H56" s="2"/>
       <c r="I56" s="2"/>
@@ -1977,20 +2005,20 @@
     </row>
     <row r="57" spans="1:13">
       <c r="A57" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B57">
         <v>0.436493528114902</v>
       </c>
       <c r="D57" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="E57" s="2">
         <v>0.39939121024477803</v>
       </c>
       <c r="F57" s="2"/>
       <c r="G57" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="H57" s="2"/>
       <c r="I57" s="2"/>
@@ -2001,13 +2029,13 @@
     </row>
     <row r="58" spans="1:13">
       <c r="A58" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B58">
         <v>41</v>
       </c>
       <c r="D58" s="3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E58" s="2">
         <v>50</v>
@@ -2036,20 +2064,20 @@
     </row>
     <row r="60" spans="1:13">
       <c r="A60" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B60">
         <v>300</v>
       </c>
       <c r="D60" s="3" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E60" s="2">
         <v>300</v>
       </c>
       <c r="F60" s="2"/>
       <c r="G60" s="3" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="H60" s="2">
         <v>300</v>
@@ -2062,20 +2090,20 @@
     </row>
     <row r="61" spans="1:13">
       <c r="A61" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B61">
         <v>72</v>
       </c>
       <c r="D61" s="3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E61" s="2">
         <v>114</v>
       </c>
       <c r="F61" s="2"/>
       <c r="G61" s="3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="H61" s="2"/>
       <c r="I61" s="2"/>
@@ -2086,20 +2114,20 @@
     </row>
     <row r="62" spans="1:13" s="1" customFormat="1">
       <c r="A62" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B62" s="1">
         <v>0.48739978480253898</v>
       </c>
       <c r="D62" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="E62" s="3">
         <v>0.48872736622167701</v>
       </c>
       <c r="F62" s="3"/>
       <c r="G62" s="9" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="H62" s="3"/>
       <c r="I62" s="3"/>
@@ -2110,20 +2138,20 @@
     </row>
     <row r="63" spans="1:13">
       <c r="A63" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B63">
         <v>0.55180492935180403</v>
       </c>
       <c r="D63" s="3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="E63" s="2">
         <v>0.62970937814422201</v>
       </c>
       <c r="F63" s="2"/>
       <c r="G63" s="3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="H63" s="2"/>
       <c r="I63" s="2"/>
@@ -2134,20 +2162,20 @@
     </row>
     <row r="64" spans="1:13">
       <c r="A64" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B64">
         <v>0.43645765496236999</v>
       </c>
       <c r="D64" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="E64" s="2">
         <v>0.39932482681408199</v>
       </c>
       <c r="F64" s="2"/>
       <c r="G64" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="H64" s="2"/>
       <c r="I64" s="2"/>
@@ -2158,13 +2186,13 @@
     </row>
     <row r="65" spans="1:13">
       <c r="A65" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B65">
         <v>41</v>
       </c>
       <c r="D65" s="3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E65" s="2">
         <v>50</v>
@@ -2193,7 +2221,7 @@
     </row>
     <row r="67" spans="1:13" s="5" customFormat="1">
       <c r="A67" s="4" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D67" s="6"/>
       <c r="E67" s="6"/>
@@ -2208,15 +2236,15 @@
     </row>
     <row r="68" spans="1:13" s="7" customFormat="1">
       <c r="A68" s="7" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D68" s="8" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E68" s="8"/>
       <c r="F68" s="8"/>
       <c r="G68" s="8" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="H68" s="8"/>
       <c r="I68" s="8"/>
@@ -2227,20 +2255,20 @@
     </row>
     <row r="69" spans="1:13" s="11" customFormat="1" ht="30">
       <c r="A69" s="10" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B69" s="11">
         <v>49.784075200442302</v>
       </c>
       <c r="D69" s="10" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E69" s="12">
         <v>26</v>
       </c>
       <c r="F69" s="12"/>
       <c r="G69" s="10" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="H69" s="12">
         <v>79.611685183746403</v>
@@ -2253,17 +2281,17 @@
     </row>
     <row r="70" spans="1:13" s="11" customFormat="1" ht="30">
       <c r="A70" s="10" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D70" s="10" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E70" s="12">
         <v>1575</v>
       </c>
       <c r="F70" s="12"/>
       <c r="G70" s="10" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="H70" s="12">
         <v>2812</v>
@@ -2293,7 +2321,7 @@
       <c r="F72" s="16"/>
       <c r="G72" s="16"/>
       <c r="H72" s="16" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="I72" s="16"/>
       <c r="J72" s="16"/>
@@ -2303,20 +2331,20 @@
     </row>
     <row r="73" spans="1:13">
       <c r="A73" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B73">
         <v>3167</v>
       </c>
       <c r="D73" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E73">
         <v>1550</v>
       </c>
       <c r="F73" s="2"/>
       <c r="G73" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="H73" s="2"/>
       <c r="I73" s="2"/>
@@ -2327,20 +2355,20 @@
     </row>
     <row r="74" spans="1:13" s="1" customFormat="1">
       <c r="A74" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B74" s="1">
         <v>0.49337237131233402</v>
       </c>
       <c r="D74" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E74" s="1">
         <v>0.39384079605051497</v>
       </c>
       <c r="F74" s="3"/>
       <c r="G74" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="H74" s="3"/>
       <c r="I74" s="3"/>
@@ -2351,20 +2379,20 @@
     </row>
     <row r="75" spans="1:13">
       <c r="A75" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B75">
         <v>0.51179921584639299</v>
       </c>
       <c r="D75" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E75">
         <v>0.49120715090927503</v>
       </c>
       <c r="F75" s="2"/>
       <c r="G75" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H75" s="2"/>
       <c r="I75" s="2"/>
@@ -2375,20 +2403,20 @@
     </row>
     <row r="76" spans="1:13">
       <c r="A76" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B76">
         <v>0.47622629596279598</v>
       </c>
       <c r="D76" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E76">
         <v>0.32868862333069199</v>
       </c>
       <c r="F76" s="2"/>
       <c r="G76" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="H76" s="2"/>
       <c r="I76" s="2"/>
@@ -2399,20 +2427,20 @@
     </row>
     <row r="77" spans="1:13">
       <c r="A77" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B77">
         <v>23</v>
       </c>
       <c r="D77" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E77">
         <v>23</v>
       </c>
       <c r="F77" s="2"/>
       <c r="G77" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="H77" s="2"/>
       <c r="I77" s="2"/>
@@ -2423,20 +2451,20 @@
     </row>
     <row r="78" spans="1:13">
       <c r="A78" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B78" s="13">
         <v>0.2</v>
       </c>
       <c r="D78" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E78" s="13">
         <v>0.2</v>
       </c>
       <c r="F78" s="2"/>
       <c r="G78" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="H78" s="2"/>
       <c r="I78" s="2"/>
@@ -2447,20 +2475,20 @@
     </row>
     <row r="79" spans="1:13" s="11" customFormat="1" ht="30">
       <c r="A79" s="10" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B79" s="11">
         <v>0</v>
       </c>
       <c r="D79" s="10" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E79" s="11">
         <v>26</v>
       </c>
       <c r="F79" s="12"/>
       <c r="G79" s="10" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="H79" s="12">
         <v>5</v>
@@ -2473,7 +2501,7 @@
     </row>
     <row r="80" spans="1:13">
       <c r="G80" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="H80">
         <v>10</v>
@@ -2494,20 +2522,20 @@
     </row>
     <row r="82" spans="1:13">
       <c r="A82" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B82">
         <v>784</v>
       </c>
       <c r="D82" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E82" s="2">
         <v>1150</v>
       </c>
       <c r="F82" s="2"/>
       <c r="G82" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="H82" s="2"/>
       <c r="I82" s="2"/>
@@ -2518,20 +2546,20 @@
     </row>
     <row r="83" spans="1:13" s="1" customFormat="1">
       <c r="A83" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B83" s="1">
         <v>0.490722548118881</v>
       </c>
       <c r="D83" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E83" s="3">
         <v>0.39386850516520699</v>
       </c>
       <c r="F83" s="3"/>
       <c r="G83" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="H83" s="3"/>
       <c r="I83" s="3"/>
@@ -2542,20 +2570,20 @@
     </row>
     <row r="84" spans="1:13">
       <c r="A84" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B84">
         <v>0.53130340451447799</v>
       </c>
       <c r="D84" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E84" s="2">
         <v>0.49129336659196898</v>
       </c>
       <c r="F84" s="2"/>
       <c r="G84" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H84" s="2"/>
       <c r="I84" s="2"/>
@@ -2566,20 +2594,20 @@
     </row>
     <row r="85" spans="1:13">
       <c r="A85" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B85">
         <v>0.45590091965929802</v>
       </c>
       <c r="D85" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E85" s="2">
         <v>0.32868862333069199</v>
       </c>
       <c r="F85" s="2"/>
       <c r="G85" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="H85" s="2"/>
       <c r="I85" s="2"/>
@@ -2590,20 +2618,20 @@
     </row>
     <row r="86" spans="1:13">
       <c r="A86" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B86">
         <v>27</v>
       </c>
       <c r="D86" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E86" s="2">
         <v>23</v>
       </c>
       <c r="F86" s="2"/>
       <c r="G86" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="H86" s="2"/>
       <c r="I86" s="2"/>
@@ -2614,20 +2642,20 @@
     </row>
     <row r="87" spans="1:13">
       <c r="A87" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B87" s="13">
         <v>0.2</v>
       </c>
       <c r="D87" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E87" s="14">
         <v>0.2</v>
       </c>
       <c r="F87" s="2"/>
       <c r="G87" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="H87" s="2"/>
       <c r="I87" s="2"/>
@@ -2638,20 +2666,20 @@
     </row>
     <row r="88" spans="1:13">
       <c r="A88" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B88">
         <v>49</v>
       </c>
       <c r="D88" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E88" s="2">
         <v>50</v>
       </c>
       <c r="F88" s="2"/>
       <c r="G88" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="H88" s="2"/>
       <c r="I88" s="2"/>
@@ -2688,17 +2716,17 @@
     </row>
     <row r="91" spans="1:13">
       <c r="A91" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D91" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E91" s="2">
         <v>5522</v>
       </c>
       <c r="F91" s="2"/>
       <c r="G91" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="H91" s="2"/>
       <c r="I91" s="2"/>
@@ -2709,15 +2737,15 @@
     </row>
     <row r="92" spans="1:13" s="1" customFormat="1">
       <c r="A92" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D92" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E92" s="3"/>
       <c r="F92" s="3"/>
       <c r="G92" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="H92" s="3"/>
       <c r="I92" s="3"/>
@@ -2728,15 +2756,15 @@
     </row>
     <row r="93" spans="1:13">
       <c r="A93" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D93" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E93" s="2"/>
       <c r="F93" s="2"/>
       <c r="G93" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H93" s="2"/>
       <c r="I93" s="2"/>
@@ -2747,15 +2775,15 @@
     </row>
     <row r="94" spans="1:13">
       <c r="A94" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D94" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E94" s="2"/>
       <c r="F94" s="2"/>
       <c r="G94" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="H94" s="2"/>
       <c r="I94" s="2"/>
@@ -2766,15 +2794,15 @@
     </row>
     <row r="95" spans="1:13">
       <c r="A95" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D95" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E95" s="2"/>
       <c r="F95" s="2"/>
       <c r="G95" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="H95" s="2"/>
       <c r="I95" s="2"/>
@@ -2785,16 +2813,16 @@
     </row>
     <row r="96" spans="1:13">
       <c r="A96" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B96" s="13"/>
       <c r="D96" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E96" s="14"/>
       <c r="F96" s="2"/>
       <c r="G96" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="H96" s="2"/>
       <c r="I96" s="2"/>
@@ -2805,20 +2833,20 @@
     </row>
     <row r="97" spans="1:13">
       <c r="A97" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B97">
         <v>100</v>
       </c>
       <c r="D97" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="E97" s="2">
         <v>5</v>
       </c>
       <c r="F97" s="2"/>
       <c r="G97" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="H97" s="2"/>
       <c r="I97" s="2"/>
@@ -2830,7 +2858,7 @@
     <row r="98" spans="1:13">
       <c r="A98" s="1"/>
       <c r="D98" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E98" s="2">
         <v>5</v>
@@ -2846,36 +2874,36 @@
     </row>
     <row r="100" spans="1:13" s="4" customFormat="1">
       <c r="A100" s="4" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="101" spans="1:13" s="7" customFormat="1">
       <c r="A101" s="7" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D101" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="G101" s="7" t="s">
         <v>6</v>
-      </c>
-      <c r="G101" s="7" t="s">
-        <v>7</v>
       </c>
     </row>
     <row r="102" spans="1:13" s="1" customFormat="1">
       <c r="A102" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B102" s="1">
         <v>2</v>
       </c>
       <c r="D102" s="3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E102" s="3">
         <v>2</v>
       </c>
       <c r="F102" s="3"/>
       <c r="G102" s="3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="H102" s="3">
         <v>2</v>
@@ -2888,15 +2916,15 @@
     </row>
     <row r="103" spans="1:13">
       <c r="A103" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D103" s="2" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E103" s="2"/>
       <c r="F103" s="2"/>
       <c r="G103" s="2" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H103" s="2"/>
       <c r="I103" s="2"/>
@@ -2907,15 +2935,15 @@
     </row>
     <row r="104" spans="1:13">
       <c r="A104" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D104" s="2" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E104" s="2"/>
       <c r="F104" s="2"/>
       <c r="G104" s="2" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="H104" s="2"/>
       <c r="I104" s="2"/>
@@ -2926,15 +2954,15 @@
     </row>
     <row r="105" spans="1:13">
       <c r="A105" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D105" s="2" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="E105" s="2"/>
       <c r="F105" s="2"/>
       <c r="G105" s="2" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="H105" s="2"/>
       <c r="I105" s="2"/>
@@ -2945,15 +2973,15 @@
     </row>
     <row r="106" spans="1:13">
       <c r="A106" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D106" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E106" s="2"/>
       <c r="F106" s="2"/>
       <c r="G106" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="H106" s="2"/>
       <c r="I106" s="2"/>
@@ -2976,20 +3004,20 @@
     </row>
     <row r="109" spans="1:13" s="1" customFormat="1">
       <c r="A109" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B109" s="1">
         <v>3</v>
       </c>
       <c r="D109" s="3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E109" s="3">
         <v>3</v>
       </c>
       <c r="F109" s="3"/>
       <c r="G109" s="3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="H109" s="3">
         <v>3</v>
@@ -3002,15 +3030,15 @@
     </row>
     <row r="110" spans="1:13">
       <c r="A110" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D110" s="2" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E110" s="2"/>
       <c r="F110" s="2"/>
       <c r="G110" s="2" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H110" s="2"/>
       <c r="I110" s="2"/>
@@ -3021,15 +3049,15 @@
     </row>
     <row r="111" spans="1:13">
       <c r="A111" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D111" s="2" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E111" s="2"/>
       <c r="F111" s="2"/>
       <c r="G111" s="2" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="H111" s="2"/>
       <c r="I111" s="2"/>
@@ -3040,15 +3068,15 @@
     </row>
     <row r="112" spans="1:13">
       <c r="A112" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D112" s="2" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="E112" s="2"/>
       <c r="F112" s="2"/>
       <c r="G112" s="2" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="H112" s="2"/>
       <c r="I112" s="2"/>
@@ -3059,15 +3087,15 @@
     </row>
     <row r="113" spans="1:13">
       <c r="A113" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D113" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E113" s="2"/>
       <c r="F113" s="2"/>
       <c r="G113" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="H113" s="2"/>
       <c r="I113" s="2"/>
@@ -3090,21 +3118,21 @@
     </row>
     <row r="116" spans="1:13" s="1" customFormat="1">
       <c r="A116" s="3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B116" s="3">
         <v>4</v>
       </c>
       <c r="C116" s="3"/>
       <c r="D116" s="3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E116" s="3">
         <v>4</v>
       </c>
       <c r="F116" s="3"/>
       <c r="G116" s="3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="H116" s="3">
         <v>4</v>
@@ -3117,21 +3145,21 @@
     </row>
     <row r="117" spans="1:13">
       <c r="A117" s="2" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B117" s="2">
         <v>3902</v>
       </c>
       <c r="C117" s="2"/>
       <c r="D117" s="2" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E117" s="2">
         <v>4285</v>
       </c>
       <c r="F117" s="2"/>
       <c r="G117" s="2" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H117" s="2"/>
       <c r="I117" s="2"/>
@@ -3142,21 +3170,21 @@
     </row>
     <row r="118" spans="1:13" s="1" customFormat="1">
       <c r="A118" s="3" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B118" s="3">
         <v>0.27126315160063702</v>
       </c>
       <c r="C118" s="3"/>
       <c r="D118" s="3" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E118" s="3">
         <v>0.38421011587133003</v>
       </c>
       <c r="F118" s="3"/>
       <c r="G118" s="3" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="H118" s="3"/>
       <c r="I118" s="3"/>
@@ -3167,21 +3195,21 @@
     </row>
     <row r="119" spans="1:13">
       <c r="A119" s="2" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B119" s="2">
         <v>0.98857203560338303</v>
       </c>
       <c r="C119" s="2"/>
       <c r="D119" s="2" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="E119" s="2">
         <v>0.53130146903195996</v>
       </c>
       <c r="F119" s="2"/>
       <c r="G119" s="2" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="H119" s="2"/>
       <c r="I119" s="2"/>
@@ -3192,21 +3220,21 @@
     </row>
     <row r="120" spans="1:13">
       <c r="A120" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B120" s="2">
         <v>0.176799337860297</v>
       </c>
       <c r="C120" s="2"/>
       <c r="D120" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E120" s="2">
         <v>0.30090442042062998</v>
       </c>
       <c r="F120" s="2"/>
       <c r="G120" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="H120" s="2"/>
       <c r="I120" s="2"/>
@@ -3217,12 +3245,12 @@
     </row>
     <row r="121" spans="1:13">
       <c r="A121" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B121" s="2"/>
       <c r="C121" s="2"/>
       <c r="D121" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E121" s="2">
         <v>53</v>
@@ -3238,14 +3266,14 @@
     </row>
     <row r="122" spans="1:13">
       <c r="A122" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B122" s="2">
         <v>0</v>
       </c>
       <c r="C122" s="2"/>
       <c r="D122" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E122" s="2">
         <v>1</v>
@@ -3261,21 +3289,21 @@
     </row>
     <row r="124" spans="1:13" s="1" customFormat="1">
       <c r="A124" s="3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B124" s="3">
         <v>5</v>
       </c>
       <c r="C124" s="3"/>
       <c r="D124" s="3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E124" s="3">
         <v>5</v>
       </c>
       <c r="F124" s="3"/>
       <c r="G124" s="3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="H124" s="3">
         <v>5</v>
@@ -3288,17 +3316,17 @@
     </row>
     <row r="125" spans="1:13">
       <c r="A125" s="2" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B125" s="2"/>
       <c r="C125" s="2"/>
       <c r="D125" s="2" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E125" s="2"/>
       <c r="F125" s="2"/>
       <c r="G125" s="2" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H125" s="2"/>
       <c r="I125" s="2"/>
@@ -3309,17 +3337,17 @@
     </row>
     <row r="126" spans="1:13">
       <c r="A126" s="2" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B126" s="2"/>
       <c r="C126" s="2"/>
       <c r="D126" s="2" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E126" s="2"/>
       <c r="F126" s="2"/>
       <c r="G126" s="2" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="H126" s="2"/>
       <c r="I126" s="2"/>
@@ -3330,17 +3358,17 @@
     </row>
     <row r="127" spans="1:13">
       <c r="A127" s="2" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B127" s="2"/>
       <c r="C127" s="2"/>
       <c r="D127" s="2" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="E127" s="2"/>
       <c r="F127" s="2"/>
       <c r="G127" s="2" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="H127" s="2"/>
       <c r="I127" s="2"/>
@@ -3351,17 +3379,17 @@
     </row>
     <row r="128" spans="1:13">
       <c r="A128" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B128" s="2"/>
       <c r="C128" s="2"/>
       <c r="D128" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E128" s="2"/>
       <c r="F128" s="2"/>
       <c r="G128" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="H128" s="2"/>
       <c r="I128" s="2"/>
@@ -3372,6 +3400,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>
@@ -3384,8 +3413,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M25"/>
   <sheetViews>
-    <sheetView showRuler="0" topLeftCell="A8" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
-      <selection activeCell="E12" sqref="E12"/>
+    <sheetView showRuler="0" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -3397,41 +3426,41 @@
   <sheetData>
     <row r="1" spans="1:13" s="4" customFormat="1">
       <c r="A1" s="4" t="s">
-        <v>0</v>
+        <v>33</v>
       </c>
     </row>
     <row r="2" spans="1:13" s="7" customFormat="1">
       <c r="A2" s="7" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D2" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="G2" s="7" t="s">
         <v>6</v>
-      </c>
-      <c r="G2" s="7" t="s">
-        <v>7</v>
       </c>
     </row>
     <row r="3" spans="1:13" s="1" customFormat="1">
       <c r="G3" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="4" spans="1:13">
       <c r="A4" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B4">
         <v>0</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E4" s="2">
         <v>0</v>
       </c>
       <c r="F4" s="2"/>
       <c r="G4" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="H4" s="2">
         <v>0</v>
@@ -3444,20 +3473,20 @@
     </row>
     <row r="5" spans="1:13">
       <c r="A5" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B5">
         <v>3902</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E5" s="2">
         <v>10057</v>
       </c>
       <c r="F5" s="2"/>
       <c r="G5" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="H5" s="2"/>
       <c r="I5" s="2"/>
@@ -3468,17 +3497,20 @@
     </row>
     <row r="6" spans="1:13" s="1" customFormat="1">
       <c r="A6" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B6" s="1">
         <v>0.49603097992439599</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
+      </c>
+      <c r="E6" s="1">
+        <v>0.47962773378500001</v>
       </c>
       <c r="F6" s="3"/>
       <c r="G6" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="H6" s="3"/>
       <c r="I6" s="3"/>
@@ -3489,17 +3521,20 @@
     </row>
     <row r="7" spans="1:13">
       <c r="A7" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B7">
         <v>0.56906542548785199</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
+      </c>
+      <c r="E7">
+        <v>0.62230621829199995</v>
       </c>
       <c r="F7" s="2"/>
       <c r="G7" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="H7" s="2"/>
       <c r="I7" s="2"/>
@@ -3510,17 +3545,20 @@
     </row>
     <row r="8" spans="1:13">
       <c r="A8" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B8">
         <v>0.440324575707433</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
+      </c>
+      <c r="E8">
+        <v>0.39039074705999999</v>
       </c>
       <c r="F8" s="2"/>
       <c r="G8" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="H8" s="2"/>
       <c r="I8" s="2"/>
@@ -3531,17 +3569,20 @@
     </row>
     <row r="9" spans="1:13">
       <c r="A9" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B9">
         <v>42</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
+      </c>
+      <c r="E9">
+        <v>50</v>
       </c>
       <c r="F9" s="2"/>
       <c r="G9" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="H9" s="2"/>
       <c r="I9" s="2"/>
@@ -3552,20 +3593,20 @@
     </row>
     <row r="12" spans="1:13">
       <c r="A12" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B12">
         <v>10</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E12" s="2">
         <v>10</v>
       </c>
       <c r="F12" s="2"/>
       <c r="G12" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="H12" s="2">
         <v>10</v>
@@ -3578,20 +3619,20 @@
     </row>
     <row r="13" spans="1:13">
       <c r="A13" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B13">
         <v>557</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E13" s="2">
         <v>1162</v>
       </c>
       <c r="F13" s="2"/>
       <c r="G13" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="H13" s="2"/>
       <c r="I13" s="2"/>
@@ -3602,20 +3643,20 @@
     </row>
     <row r="14" spans="1:13" s="1" customFormat="1">
       <c r="A14" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B14" s="1">
         <v>0.49370813828154803</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="E14" s="3">
         <v>0.479631648691</v>
       </c>
       <c r="F14" s="3"/>
       <c r="G14" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="H14" s="3"/>
       <c r="I14" s="3"/>
@@ -3626,20 +3667,20 @@
     </row>
     <row r="15" spans="1:13">
       <c r="A15" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B15">
         <v>0.57207093873627302</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="E15" s="2">
         <v>0.62231917582200003</v>
       </c>
       <c r="F15" s="2"/>
       <c r="G15" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="H15" s="2"/>
       <c r="I15" s="2"/>
@@ -3650,20 +3691,20 @@
     </row>
     <row r="16" spans="1:13">
       <c r="A16" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B16">
         <v>0.43487591306479301</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="E16" s="2">
         <v>0.39039074705999999</v>
       </c>
       <c r="F16" s="2"/>
       <c r="G16" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="H16" s="2"/>
       <c r="I16" s="2"/>
@@ -3674,20 +3715,20 @@
     </row>
     <row r="17" spans="1:13">
       <c r="A17" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B17">
         <v>44.2</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="E17" s="2">
         <v>50</v>
       </c>
       <c r="F17" s="2"/>
       <c r="G17" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="H17" s="2"/>
       <c r="I17" s="2"/>
@@ -3698,20 +3739,20 @@
     </row>
     <row r="20" spans="1:13">
       <c r="A20" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B20">
         <v>100</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E20" s="2">
         <v>100</v>
       </c>
       <c r="F20" s="2"/>
       <c r="G20" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="H20" s="2">
         <v>100</v>
@@ -3724,18 +3765,18 @@
     </row>
     <row r="21" spans="1:13">
       <c r="A21" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B21">
         <v>152</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E21" s="2"/>
       <c r="F21" s="2"/>
       <c r="G21" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="H21" s="2"/>
       <c r="I21" s="2"/>
@@ -3746,18 +3787,18 @@
     </row>
     <row r="22" spans="1:13" s="1" customFormat="1">
       <c r="A22" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B22" s="1">
         <v>0.49402044410599999</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="E22" s="3"/>
       <c r="F22" s="3"/>
       <c r="G22" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="H22" s="3"/>
       <c r="I22" s="3"/>
@@ -3768,18 +3809,18 @@
     </row>
     <row r="23" spans="1:13">
       <c r="A23" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B23">
         <v>0.56804575176399996</v>
       </c>
       <c r="D23" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="E23" s="2"/>
       <c r="F23" s="2"/>
       <c r="G23" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="H23" s="2"/>
       <c r="I23" s="2"/>
@@ -3790,18 +3831,18 @@
     </row>
     <row r="24" spans="1:13">
       <c r="A24" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B24">
         <v>0.43758762674099999</v>
       </c>
       <c r="D24" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="E24" s="2"/>
       <c r="F24" s="2"/>
       <c r="G24" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="H24" s="2"/>
       <c r="I24" s="2"/>
@@ -3812,18 +3853,18 @@
     </row>
     <row r="25" spans="1:13">
       <c r="A25" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B25">
         <v>42.799999999999898</v>
       </c>
       <c r="D25" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="E25" s="2"/>
       <c r="F25" s="2"/>
       <c r="G25" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="H25" s="2"/>
       <c r="I25" s="2"/>
@@ -3834,6 +3875,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>
@@ -3844,12 +3886,760 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:M9"/>
   <sheetViews>
-    <sheetView showRuler="0" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0"/>
+    <sheetView showRuler="0" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="16.6640625" customWidth="1"/>
+    <col min="4" max="4" width="15.6640625" customWidth="1"/>
+    <col min="7" max="7" width="15.83203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:13" s="4" customFormat="1">
+      <c r="A1" s="4" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" s="7" customFormat="1">
+      <c r="A2" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="D2" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="G2" s="7" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" s="1" customFormat="1">
+      <c r="G3" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13">
+      <c r="A4" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B4">
+        <v>1</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E4" s="2">
+        <v>1</v>
+      </c>
+      <c r="F4" s="2"/>
+      <c r="G4" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="H4" s="2">
+        <v>1</v>
+      </c>
+      <c r="I4" s="2"/>
+      <c r="J4" s="2"/>
+      <c r="K4" s="2"/>
+      <c r="L4" s="2"/>
+      <c r="M4" s="2"/>
+    </row>
+    <row r="5" spans="1:13">
+      <c r="A5" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B5">
+        <v>1729</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E5" s="2"/>
+      <c r="F5" s="2"/>
+      <c r="G5" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="H5" s="2"/>
+      <c r="I5" s="2"/>
+      <c r="J5" s="2"/>
+      <c r="K5" s="2"/>
+      <c r="L5" s="2"/>
+      <c r="M5" s="2"/>
+    </row>
+    <row r="6" spans="1:13" s="1" customFormat="1">
+      <c r="A6" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B6" s="1">
+        <v>0.51408817950591101</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="E6" s="3"/>
+      <c r="F6" s="3"/>
+      <c r="G6" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="H6" s="3"/>
+      <c r="I6" s="3"/>
+      <c r="J6" s="3"/>
+      <c r="K6" s="3"/>
+      <c r="L6" s="3"/>
+      <c r="M6" s="3"/>
+    </row>
+    <row r="7" spans="1:13">
+      <c r="A7" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B7">
+        <v>0.53505107641116001</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="E7" s="2"/>
+      <c r="F7" s="2"/>
+      <c r="G7" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="H7" s="2"/>
+      <c r="I7" s="2"/>
+      <c r="J7" s="2"/>
+      <c r="K7" s="2"/>
+      <c r="L7" s="2"/>
+      <c r="M7" s="2"/>
+    </row>
+    <row r="8" spans="1:13">
+      <c r="A8" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B8">
+        <v>0.49470597325862897</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="E8" s="2"/>
+      <c r="F8" s="2"/>
+      <c r="G8" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="H8" s="2"/>
+      <c r="I8" s="2"/>
+      <c r="J8" s="2"/>
+      <c r="K8" s="2"/>
+      <c r="L8" s="2"/>
+      <c r="M8" s="2"/>
+    </row>
+    <row r="9" spans="1:13">
+      <c r="A9" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B9">
+        <v>29</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="E9" s="2"/>
+      <c r="F9" s="2"/>
+      <c r="G9" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="H9" s="2"/>
+      <c r="I9" s="2"/>
+      <c r="J9" s="2"/>
+      <c r="K9" s="2"/>
+      <c r="L9" s="2"/>
+      <c r="M9" s="2"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:M25"/>
+  <sheetViews>
+    <sheetView showRuler="0" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
+      <selection sqref="A1:XFD1048576"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <cols>
+    <col min="1" max="1" width="15" customWidth="1"/>
+    <col min="4" max="4" width="13.6640625" customWidth="1"/>
+    <col min="7" max="7" width="16" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:13" s="4" customFormat="1">
+      <c r="A1" s="4" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" s="7" customFormat="1">
+      <c r="A2" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="D2" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="G2" s="7" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" s="1" customFormat="1">
+      <c r="G3" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13">
+      <c r="A4" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B4">
+        <v>1</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E4" s="2">
+        <v>1</v>
+      </c>
+      <c r="F4" s="2"/>
+      <c r="G4" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="H4" s="2">
+        <v>1</v>
+      </c>
+      <c r="I4" s="2"/>
+      <c r="J4" s="2"/>
+      <c r="K4" s="2"/>
+      <c r="L4" s="2"/>
+      <c r="M4" s="2"/>
+    </row>
+    <row r="5" spans="1:13">
+      <c r="A5" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E5" s="2"/>
+      <c r="F5" s="2"/>
+      <c r="G5" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="H5" s="2"/>
+      <c r="I5" s="2"/>
+      <c r="J5" s="2"/>
+      <c r="K5" s="2"/>
+      <c r="L5" s="2"/>
+      <c r="M5" s="2"/>
+    </row>
+    <row r="6" spans="1:13" s="1" customFormat="1">
+      <c r="A6" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="F6" s="3"/>
+      <c r="G6" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="H6" s="3"/>
+      <c r="I6" s="3"/>
+      <c r="J6" s="3"/>
+      <c r="K6" s="3"/>
+      <c r="L6" s="3"/>
+      <c r="M6" s="3"/>
+    </row>
+    <row r="7" spans="1:13">
+      <c r="A7" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="F7" s="2"/>
+      <c r="G7" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="H7" s="2"/>
+      <c r="I7" s="2"/>
+      <c r="J7" s="2"/>
+      <c r="K7" s="2"/>
+      <c r="L7" s="2"/>
+      <c r="M7" s="2"/>
+    </row>
+    <row r="8" spans="1:13">
+      <c r="A8" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="F8" s="2"/>
+      <c r="G8" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="H8" s="2"/>
+      <c r="I8" s="2"/>
+      <c r="J8" s="2"/>
+      <c r="K8" s="2"/>
+      <c r="L8" s="2"/>
+      <c r="M8" s="2"/>
+    </row>
+    <row r="9" spans="1:13">
+      <c r="A9" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="F9" s="2"/>
+      <c r="G9" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="H9" s="2"/>
+      <c r="I9" s="2"/>
+      <c r="J9" s="2"/>
+      <c r="K9" s="2"/>
+      <c r="L9" s="2"/>
+      <c r="M9" s="2"/>
+    </row>
+    <row r="12" spans="1:13">
+      <c r="A12" s="1"/>
+      <c r="D12" s="1"/>
+      <c r="E12" s="2"/>
+      <c r="F12" s="2"/>
+      <c r="G12" s="1"/>
+      <c r="H12" s="2"/>
+      <c r="I12" s="2"/>
+      <c r="J12" s="2"/>
+      <c r="K12" s="2"/>
+      <c r="L12" s="2"/>
+      <c r="M12" s="2"/>
+    </row>
+    <row r="13" spans="1:13">
+      <c r="A13" s="1"/>
+      <c r="D13" s="1"/>
+      <c r="E13" s="2"/>
+      <c r="F13" s="2"/>
+      <c r="G13" s="1"/>
+      <c r="H13" s="2"/>
+      <c r="I13" s="2"/>
+      <c r="J13" s="2"/>
+      <c r="K13" s="2"/>
+      <c r="L13" s="2"/>
+      <c r="M13" s="2"/>
+    </row>
+    <row r="14" spans="1:13" s="1" customFormat="1">
+      <c r="E14" s="3"/>
+      <c r="F14" s="3"/>
+      <c r="H14" s="3"/>
+      <c r="I14" s="3"/>
+      <c r="J14" s="3"/>
+      <c r="K14" s="3"/>
+      <c r="L14" s="3"/>
+      <c r="M14" s="3"/>
+    </row>
+    <row r="15" spans="1:13">
+      <c r="A15" s="1"/>
+      <c r="D15" s="1"/>
+      <c r="E15" s="2"/>
+      <c r="F15" s="2"/>
+      <c r="G15" s="1"/>
+      <c r="H15" s="2"/>
+      <c r="I15" s="2"/>
+      <c r="J15" s="2"/>
+      <c r="K15" s="2"/>
+      <c r="L15" s="2"/>
+      <c r="M15" s="2"/>
+    </row>
+    <row r="16" spans="1:13">
+      <c r="A16" s="1"/>
+      <c r="D16" s="1"/>
+      <c r="E16" s="2"/>
+      <c r="F16" s="2"/>
+      <c r="G16" s="1"/>
+      <c r="H16" s="2"/>
+      <c r="I16" s="2"/>
+      <c r="J16" s="2"/>
+      <c r="K16" s="2"/>
+      <c r="L16" s="2"/>
+      <c r="M16" s="2"/>
+    </row>
+    <row r="17" spans="1:13">
+      <c r="A17" s="1"/>
+      <c r="D17" s="1"/>
+      <c r="E17" s="2"/>
+      <c r="F17" s="2"/>
+      <c r="G17" s="1"/>
+      <c r="H17" s="2"/>
+      <c r="I17" s="2"/>
+      <c r="J17" s="2"/>
+      <c r="K17" s="2"/>
+      <c r="L17" s="2"/>
+      <c r="M17" s="2"/>
+    </row>
+    <row r="20" spans="1:13">
+      <c r="A20" s="1"/>
+      <c r="D20" s="1"/>
+      <c r="E20" s="2"/>
+      <c r="F20" s="2"/>
+      <c r="G20" s="1"/>
+      <c r="H20" s="2"/>
+      <c r="I20" s="2"/>
+      <c r="J20" s="2"/>
+      <c r="K20" s="2"/>
+      <c r="L20" s="2"/>
+      <c r="M20" s="2"/>
+    </row>
+    <row r="21" spans="1:13">
+      <c r="A21" s="1"/>
+      <c r="D21" s="1"/>
+      <c r="E21" s="2"/>
+      <c r="F21" s="2"/>
+      <c r="G21" s="1"/>
+      <c r="H21" s="2"/>
+      <c r="I21" s="2"/>
+      <c r="J21" s="2"/>
+      <c r="K21" s="2"/>
+      <c r="L21" s="2"/>
+      <c r="M21" s="2"/>
+    </row>
+    <row r="22" spans="1:13" s="1" customFormat="1">
+      <c r="E22" s="3"/>
+      <c r="F22" s="3"/>
+      <c r="H22" s="3"/>
+      <c r="I22" s="3"/>
+      <c r="J22" s="3"/>
+      <c r="K22" s="3"/>
+      <c r="L22" s="3"/>
+      <c r="M22" s="3"/>
+    </row>
+    <row r="23" spans="1:13">
+      <c r="A23" s="1"/>
+      <c r="D23" s="1"/>
+      <c r="E23" s="2"/>
+      <c r="F23" s="2"/>
+      <c r="G23" s="1"/>
+      <c r="H23" s="2"/>
+      <c r="I23" s="2"/>
+      <c r="J23" s="2"/>
+      <c r="K23" s="2"/>
+      <c r="L23" s="2"/>
+      <c r="M23" s="2"/>
+    </row>
+    <row r="24" spans="1:13">
+      <c r="A24" s="1"/>
+      <c r="D24" s="1"/>
+      <c r="E24" s="2"/>
+      <c r="F24" s="2"/>
+      <c r="G24" s="1"/>
+      <c r="H24" s="2"/>
+      <c r="I24" s="2"/>
+      <c r="J24" s="2"/>
+      <c r="K24" s="2"/>
+      <c r="L24" s="2"/>
+      <c r="M24" s="2"/>
+    </row>
+    <row r="25" spans="1:13">
+      <c r="A25" s="1"/>
+      <c r="D25" s="1"/>
+      <c r="E25" s="2"/>
+      <c r="F25" s="2"/>
+      <c r="G25" s="1"/>
+      <c r="H25" s="2"/>
+      <c r="I25" s="2"/>
+      <c r="J25" s="2"/>
+      <c r="K25" s="2"/>
+      <c r="L25" s="2"/>
+      <c r="M25" s="2"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:M24"/>
+  <sheetViews>
+    <sheetView tabSelected="1" showRuler="0" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <cols>
+    <col min="1" max="1" width="15" customWidth="1"/>
+    <col min="4" max="4" width="13.6640625" customWidth="1"/>
+    <col min="7" max="7" width="16" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:13" s="4" customFormat="1">
+      <c r="A1" s="4" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" s="1" customFormat="1"/>
+    <row r="3" spans="1:13">
+      <c r="A3" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B3">
+        <v>0</v>
+      </c>
+      <c r="D3" s="1"/>
+      <c r="E3" s="2"/>
+      <c r="F3" s="2"/>
+      <c r="G3" s="1"/>
+      <c r="H3" s="2"/>
+      <c r="I3" s="2"/>
+      <c r="J3" s="2"/>
+      <c r="K3" s="2"/>
+      <c r="L3" s="2"/>
+      <c r="M3" s="2"/>
+    </row>
+    <row r="4" spans="1:13">
+      <c r="A4" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D4" s="1"/>
+      <c r="E4" s="2"/>
+      <c r="F4" s="2"/>
+      <c r="G4" s="1"/>
+      <c r="H4" s="2"/>
+      <c r="I4" s="2"/>
+      <c r="J4" s="2"/>
+      <c r="K4" s="2"/>
+      <c r="L4" s="2"/>
+      <c r="M4" s="2"/>
+    </row>
+    <row r="5" spans="1:13" s="1" customFormat="1">
+      <c r="A5" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="F5" s="3"/>
+      <c r="H5" s="3"/>
+      <c r="I5" s="3"/>
+      <c r="J5" s="3"/>
+      <c r="K5" s="3"/>
+      <c r="L5" s="3"/>
+      <c r="M5" s="3"/>
+    </row>
+    <row r="6" spans="1:13">
+      <c r="A6" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D6" s="1"/>
+      <c r="F6" s="2"/>
+      <c r="G6" s="1"/>
+      <c r="H6" s="2"/>
+      <c r="I6" s="2"/>
+      <c r="J6" s="2"/>
+      <c r="K6" s="2"/>
+      <c r="L6" s="2"/>
+      <c r="M6" s="2"/>
+    </row>
+    <row r="7" spans="1:13">
+      <c r="A7" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="D7" s="1"/>
+      <c r="F7" s="2"/>
+      <c r="G7" s="1"/>
+      <c r="H7" s="2"/>
+      <c r="I7" s="2"/>
+      <c r="J7" s="2"/>
+      <c r="K7" s="2"/>
+      <c r="L7" s="2"/>
+      <c r="M7" s="2"/>
+    </row>
+    <row r="8" spans="1:13">
+      <c r="A8" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="D8" s="1"/>
+      <c r="F8" s="2"/>
+      <c r="G8" s="1"/>
+      <c r="H8" s="2"/>
+      <c r="I8" s="2"/>
+      <c r="J8" s="2"/>
+      <c r="K8" s="2"/>
+      <c r="L8" s="2"/>
+      <c r="M8" s="2"/>
+    </row>
+    <row r="11" spans="1:13">
+      <c r="A11" s="1"/>
+      <c r="D11" s="1"/>
+      <c r="E11" s="2"/>
+      <c r="F11" s="2"/>
+      <c r="G11" s="1"/>
+      <c r="H11" s="2"/>
+      <c r="I11" s="2"/>
+      <c r="J11" s="2"/>
+      <c r="K11" s="2"/>
+      <c r="L11" s="2"/>
+      <c r="M11" s="2"/>
+    </row>
+    <row r="12" spans="1:13">
+      <c r="A12" s="1"/>
+      <c r="D12" s="1"/>
+      <c r="E12" s="2"/>
+      <c r="F12" s="2"/>
+      <c r="G12" s="1"/>
+      <c r="H12" s="2"/>
+      <c r="I12" s="2"/>
+      <c r="J12" s="2"/>
+      <c r="K12" s="2"/>
+      <c r="L12" s="2"/>
+      <c r="M12" s="2"/>
+    </row>
+    <row r="13" spans="1:13" s="1" customFormat="1">
+      <c r="E13" s="3"/>
+      <c r="F13" s="3"/>
+      <c r="H13" s="3"/>
+      <c r="I13" s="3"/>
+      <c r="J13" s="3"/>
+      <c r="K13" s="3"/>
+      <c r="L13" s="3"/>
+      <c r="M13" s="3"/>
+    </row>
+    <row r="14" spans="1:13">
+      <c r="A14" s="1"/>
+      <c r="D14" s="1"/>
+      <c r="E14" s="2"/>
+      <c r="F14" s="2"/>
+      <c r="G14" s="1"/>
+      <c r="H14" s="2"/>
+      <c r="I14" s="2"/>
+      <c r="J14" s="2"/>
+      <c r="K14" s="2"/>
+      <c r="L14" s="2"/>
+      <c r="M14" s="2"/>
+    </row>
+    <row r="15" spans="1:13">
+      <c r="A15" s="1"/>
+      <c r="D15" s="1"/>
+      <c r="E15" s="2"/>
+      <c r="F15" s="2"/>
+      <c r="G15" s="1"/>
+      <c r="H15" s="2"/>
+      <c r="I15" s="2"/>
+      <c r="J15" s="2"/>
+      <c r="K15" s="2"/>
+      <c r="L15" s="2"/>
+      <c r="M15" s="2"/>
+    </row>
+    <row r="16" spans="1:13">
+      <c r="A16" s="1"/>
+      <c r="D16" s="1"/>
+      <c r="E16" s="2"/>
+      <c r="F16" s="2"/>
+      <c r="G16" s="1"/>
+      <c r="H16" s="2"/>
+      <c r="I16" s="2"/>
+      <c r="J16" s="2"/>
+      <c r="K16" s="2"/>
+      <c r="L16" s="2"/>
+      <c r="M16" s="2"/>
+    </row>
+    <row r="19" spans="1:13">
+      <c r="A19" s="1"/>
+      <c r="D19" s="1"/>
+      <c r="E19" s="2"/>
+      <c r="F19" s="2"/>
+      <c r="G19" s="1"/>
+      <c r="H19" s="2"/>
+      <c r="I19" s="2"/>
+      <c r="J19" s="2"/>
+      <c r="K19" s="2"/>
+      <c r="L19" s="2"/>
+      <c r="M19" s="2"/>
+    </row>
+    <row r="20" spans="1:13">
+      <c r="A20" s="1"/>
+      <c r="D20" s="1"/>
+      <c r="E20" s="2"/>
+      <c r="F20" s="2"/>
+      <c r="G20" s="1"/>
+      <c r="H20" s="2"/>
+      <c r="I20" s="2"/>
+      <c r="J20" s="2"/>
+      <c r="K20" s="2"/>
+      <c r="L20" s="2"/>
+      <c r="M20" s="2"/>
+    </row>
+    <row r="21" spans="1:13" s="1" customFormat="1">
+      <c r="E21" s="3"/>
+      <c r="F21" s="3"/>
+      <c r="H21" s="3"/>
+      <c r="I21" s="3"/>
+      <c r="J21" s="3"/>
+      <c r="K21" s="3"/>
+      <c r="L21" s="3"/>
+      <c r="M21" s="3"/>
+    </row>
+    <row r="22" spans="1:13">
+      <c r="A22" s="1"/>
+      <c r="D22" s="1"/>
+      <c r="E22" s="2"/>
+      <c r="F22" s="2"/>
+      <c r="G22" s="1"/>
+      <c r="H22" s="2"/>
+      <c r="I22" s="2"/>
+      <c r="J22" s="2"/>
+      <c r="K22" s="2"/>
+      <c r="L22" s="2"/>
+      <c r="M22" s="2"/>
+    </row>
+    <row r="23" spans="1:13">
+      <c r="A23" s="1"/>
+      <c r="D23" s="1"/>
+      <c r="E23" s="2"/>
+      <c r="F23" s="2"/>
+      <c r="G23" s="1"/>
+      <c r="H23" s="2"/>
+      <c r="I23" s="2"/>
+      <c r="J23" s="2"/>
+      <c r="K23" s="2"/>
+      <c r="L23" s="2"/>
+      <c r="M23" s="2"/>
+    </row>
+    <row r="24" spans="1:13">
+      <c r="A24" s="1"/>
+      <c r="D24" s="1"/>
+      <c r="E24" s="2"/>
+      <c r="F24" s="2"/>
+      <c r="G24" s="1"/>
+      <c r="H24" s="2"/>
+      <c r="I24" s="2"/>
+      <c r="J24" s="2"/>
+      <c r="K24" s="2"/>
+      <c r="L24" s="2"/>
+      <c r="M24" s="2"/>
+    </row>
+  </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">

</xml_diff>